<commit_message>
Mise a jour CV Trie offre de stage intranet Creation de lettre de motivations 2016 Ajout postulations 2016 au 06/01/2016
</commit_message>
<xml_diff>
--- a/offre de stage/postulation.xlsx
+++ b/offre de stage/postulation.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="2015" sheetId="1" r:id="rId1"/>
+    <sheet name="2016" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <webPublishing vml="1" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Entreprise</t>
   </si>
@@ -103,19 +104,148 @@
   </si>
   <si>
     <t>François Niarfeix via claire</t>
+  </si>
+  <si>
+    <t>Valeao</t>
+  </si>
+  <si>
+    <t>Medtech</t>
+  </si>
+  <si>
+    <t>A postuler</t>
+  </si>
+  <si>
+    <t>http://www.balyo.com/fr/Recrutement/Candidature-spontanee</t>
+  </si>
+  <si>
+    <t>http://www.arbor-technologies.com/contact/</t>
+  </si>
+  <si>
+    <t>http://mach4.fr/category/produits/</t>
+  </si>
+  <si>
+    <t>http://www.staubli.com/fr/</t>
+  </si>
+  <si>
+    <t>http://www.eos-innovation.eu/ContactFr/Index.sls</t>
+  </si>
+  <si>
+    <t>RECHERCHER SUR LINKDIN SI CONTACT ESME AVANT !!!!!</t>
+  </si>
+  <si>
+    <t>http://www.sileane.com/contact</t>
+  </si>
+  <si>
+    <t>recrutement@sileane.com</t>
+  </si>
+  <si>
+    <t>http://www.humarobotics.com/</t>
+  </si>
+  <si>
+    <t>http://www.sarrazin-technologies.com/contact/</t>
+  </si>
+  <si>
+    <t>http://www.tecdron.fr/en/contact-2/</t>
+  </si>
+  <si>
+    <t>recrutement@basystemes.fr</t>
+  </si>
+  <si>
+    <t>http://www.basystemes.com/recrutement/offres-demploi/</t>
+  </si>
+  <si>
+    <t>http://www.sellen-pharmacie.fr/contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renault </t>
+  </si>
+  <si>
+    <t>Parrot</t>
+  </si>
+  <si>
+    <t>Safran</t>
+  </si>
+  <si>
+    <t>Mise en œuvre gyrolaser</t>
+  </si>
+  <si>
+    <t>RÉGULATION D'UN ENSEMBLE PROPULSIF COMPOSÉ DE PLUSIEURS MOTEURS H/F</t>
+  </si>
+  <si>
+    <t>2015-40935 module poussée</t>
+  </si>
+  <si>
+    <t>Eosgen</t>
+  </si>
+  <si>
+    <t>Bus de terrain</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>p.maillet@medtechsurgical.com</t>
+  </si>
+  <si>
+    <t>Baylo</t>
+  </si>
+  <si>
+    <t>Candidature spontanée</t>
+  </si>
+  <si>
+    <t>Arbor technologies</t>
+  </si>
+  <si>
+    <t>En attente d'envoi</t>
+  </si>
+  <si>
+    <t>compliqué ..</t>
+  </si>
+  <si>
+    <t>Staubli</t>
+  </si>
+  <si>
+    <t>Candidature par mail contact sur site sans cv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF909090"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,14 +265,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -615,14 +754,233 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42374</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42375</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42375</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42375</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42375</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A17" r:id="rId1"/>
+    <hyperlink ref="F11" r:id="rId2"/>
+    <hyperlink ref="C24" r:id="rId3" tooltip="Postulez en ligne !" display="mailto:recrutement@basystemes.fr"/>
+    <hyperlink ref="A24" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Migration big pc 13/01/2016
</commit_message>
<xml_diff>
--- a/offre de stage/postulation.xlsx
+++ b/offre de stage/postulation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>Entreprise</t>
   </si>
@@ -332,13 +332,22 @@
   </si>
   <si>
     <t>Réponse : Robotique en milieu hostile</t>
+  </si>
+  <si>
+    <t>Tecdron</t>
+  </si>
+  <si>
+    <t>cyberdroid</t>
+  </si>
+  <si>
+    <t>naio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,7 +479,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,9 +511,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,6 +546,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,21 +722,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -745,7 +756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -756,7 +767,7 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -767,7 +778,7 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -778,7 +789,7 @@
         <v>42093</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -792,7 +803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -803,7 +814,7 @@
         <v>42100</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -817,7 +828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -831,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -842,7 +853,7 @@
         <v>42100</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -856,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -870,7 +881,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -891,21 +902,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +942,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -945,7 +956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -962,7 +973,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -976,7 +987,7 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -987,7 +998,10 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -995,7 +1009,10 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
       <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
@@ -1003,7 +1020,7 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1020,7 +1037,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1037,7 +1054,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1057,7 +1074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1074,7 +1091,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1091,7 +1108,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1108,7 +1125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1128,7 +1145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1151,7 +1168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1166,7 +1183,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1179,7 +1196,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1192,7 +1209,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1202,10 +1219,12 @@
       <c r="C20" s="1">
         <v>42379</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>42382</v>
+      </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1220,7 +1239,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1233,7 +1252,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -1248,7 +1267,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1263,7 +1282,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -1276,7 +1295,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -1292,7 +1311,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -1305,7 +1324,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1321,7 +1340,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1337,7 +1356,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>83</v>
       </c>
@@ -1353,7 +1372,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -1369,7 +1388,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>101</v>
       </c>
@@ -1383,7 +1402,7 @@
       <c r="F32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -1397,37 +1416,81 @@
       <c r="F33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="35" spans="1:9">
-      <c r="B35" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="1">
+        <v>42382</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="1">
+        <v>42382</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="1">
+        <v>42382</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1443,7 +1506,7 @@
     <hyperlink ref="I11" r:id="rId8"/>
     <hyperlink ref="F13" r:id="rId9"/>
     <hyperlink ref="F14" r:id="rId10"/>
-    <hyperlink ref="A39" r:id="rId11"/>
+    <hyperlink ref="A42" r:id="rId11"/>
     <hyperlink ref="F16" r:id="rId12"/>
     <hyperlink ref="A30" r:id="rId13" display="mailto:jobs@sen.se"/>
     <hyperlink ref="I29" r:id="rId14"/>
@@ -1458,12 +1521,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
changement pc, préparation mails
</commit_message>
<xml_diff>
--- a/offre de stage/postulation.xlsx
+++ b/offre de stage/postulation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="113">
   <si>
     <t>Entreprise</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Medtech</t>
   </si>
   <si>
-    <t>A postuler</t>
-  </si>
-  <si>
     <t>http://www.balyo.com/fr/Recrutement/Candidature-spontanee</t>
   </si>
   <si>
@@ -127,15 +124,9 @@
     <t>http://www.eos-innovation.eu/ContactFr/Index.sls</t>
   </si>
   <si>
-    <t>RECHERCHER SUR LINKDIN SI CONTACT ESME AVANT !!!!!</t>
-  </si>
-  <si>
     <t>http://www.sileane.com/contact</t>
   </si>
   <si>
-    <t>http://www.tecdron.fr/en/contact-2/</t>
-  </si>
-  <si>
     <t>recrutement@basystemes.fr</t>
   </si>
   <si>
@@ -341,13 +332,37 @@
   </si>
   <si>
     <t>naio</t>
+  </si>
+  <si>
+    <t>Thales</t>
+  </si>
+  <si>
+    <t>réponse Développement et innovation d'assemblage satellite par système robotique</t>
+  </si>
+  <si>
+    <t>Areva</t>
+  </si>
+  <si>
+    <t>STAGE: DÉVELOPPEMENT D'UN PROCÉDÉ ÉLECTROÉROSION</t>
+  </si>
+  <si>
+    <t>Plastic Omnium</t>
+  </si>
+  <si>
+    <t>Stage ingénieur mécatronique</t>
+  </si>
+  <si>
+    <t>Roboplanet</t>
+  </si>
+  <si>
+    <t>Ingénieur informatique industrielle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,14 +378,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
@@ -379,6 +386,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -414,10 +427,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -479,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,10 +524,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -546,7 +558,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -722,21 +733,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -756,7 +767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -767,7 +778,7 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -778,7 +789,7 @@
         <v>42092</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -789,7 +800,7 @@
         <v>42093</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -803,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -814,7 +825,7 @@
         <v>42100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -828,7 +839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -842,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -853,7 +864,7 @@
         <v>42100</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -867,7 +878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -881,7 +892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -902,21 +913,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -936,15 +947,15 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -953,10 +964,10 @@
         <v>42373</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -967,18 +978,18 @@
         <v>42374</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>42375</v>
@@ -987,170 +998,170 @@
         <v>42375</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>42375</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>42375</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C8" s="1">
         <v>42375</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1">
         <v>42375</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1">
         <v>42375</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
         <v>42375</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
         <v>42376</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>42376</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1">
         <v>42376</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
       </c>
       <c r="C15" s="1">
         <v>42376</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1">
         <v>42376</v>
@@ -1159,21 +1170,21 @@
         <v>42377</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
         <v>62</v>
       </c>
-      <c r="H16" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" t="s">
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
       </c>
       <c r="C17" s="1">
         <v>42379</v>
@@ -1183,12 +1194,12 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>42379</v>
@@ -1196,12 +1207,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1">
         <v>42379</v>
@@ -1209,12 +1220,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1">
         <v>42379</v>
@@ -1224,27 +1235,27 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1">
         <v>42379</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1">
         <v>42379</v>
@@ -1252,42 +1263,42 @@
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C23" s="1">
         <v>42379</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1">
         <v>42380</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1">
         <v>42380</v>
@@ -1295,12 +1306,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" s="1">
         <v>42381</v>
@@ -1308,15 +1319,15 @@
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C27" s="1">
         <v>42380</v>
@@ -1324,9 +1335,9 @@
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -1337,15 +1348,15 @@
       <c r="E28" s="1"/>
       <c r="F28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1">
         <v>42381</v>
@@ -1353,15 +1364,15 @@
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
       <c r="I29" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1">
         <v>42381</v>
@@ -1369,15 +1380,15 @@
       <c r="E30" s="1"/>
       <c r="F30" s="2"/>
       <c r="I30" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1">
         <v>42381</v>
@@ -1385,15 +1396,15 @@
       <c r="E31" s="1"/>
       <c r="F31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C32" s="1">
         <v>42381</v>
@@ -1402,12 +1413,12 @@
       <c r="F32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1">
         <v>42381</v>
@@ -1416,12 +1427,12 @@
       <c r="F33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1">
         <v>42382</v>
@@ -1430,12 +1441,12 @@
       <c r="F34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1">
         <v>42382</v>
@@ -1444,54 +1455,86 @@
       <c r="F35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
         <v>42382</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="1">
+        <v>42382</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="1">
+        <v>42382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1">
+        <v>42383</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="C41" s="1">
+        <v>42383</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1506,27 +1549,26 @@
     <hyperlink ref="I11" r:id="rId8"/>
     <hyperlink ref="F13" r:id="rId9"/>
     <hyperlink ref="F14" r:id="rId10"/>
-    <hyperlink ref="A42" r:id="rId11"/>
-    <hyperlink ref="F16" r:id="rId12"/>
-    <hyperlink ref="A30" r:id="rId13" display="mailto:jobs@sen.se"/>
-    <hyperlink ref="I29" r:id="rId14"/>
-    <hyperlink ref="I30" r:id="rId15"/>
-    <hyperlink ref="I28" r:id="rId16"/>
-    <hyperlink ref="I31" r:id="rId17"/>
-    <hyperlink ref="I26" r:id="rId18"/>
+    <hyperlink ref="F16" r:id="rId11"/>
+    <hyperlink ref="A30" r:id="rId12" display="mailto:jobs@sen.se"/>
+    <hyperlink ref="I29" r:id="rId13"/>
+    <hyperlink ref="I30" r:id="rId14"/>
+    <hyperlink ref="I28" r:id="rId15"/>
+    <hyperlink ref="I31" r:id="rId16"/>
+    <hyperlink ref="I26" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
commit pour rdv ait
</commit_message>
<xml_diff>
--- a/offre de stage/postulation.xlsx
+++ b/offre de stage/postulation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
   <si>
     <t>Entreprise</t>
   </si>
@@ -208,9 +208,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Robot Swin</t>
-  </si>
-  <si>
     <t>Réponse offre inégnieur mécatronique</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>Valeo</t>
   </si>
   <si>
-    <t>candidature spontanéée à M mach, attente réponse sinon ajutant</t>
-  </si>
-  <si>
     <t xml:space="preserve">navya </t>
   </si>
   <si>
@@ -412,14 +406,89 @@
     <t>transfert RH le 19/01</t>
   </si>
   <si>
-    <t>Potentiel</t>
+    <t>transfert</t>
+  </si>
+  <si>
+    <t>candidature spontanéée à M mach + ajutant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bertand </t>
+  </si>
+  <si>
+    <t>Renvoi mail relance</t>
+  </si>
+  <si>
+    <t>recrutement@fr.bertrandt.com</t>
+  </si>
+  <si>
+    <t>Bitmakers</t>
+  </si>
+  <si>
+    <t>Téléphone</t>
+  </si>
+  <si>
+    <t>Avis</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Aldebaran</t>
+  </si>
+  <si>
+    <t>Stage FSR</t>
+  </si>
+  <si>
+    <t>~+</t>
+  </si>
+  <si>
+    <t>Robot Swim</t>
+  </si>
+  <si>
+    <t>SkF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidature stagiaire automatisme </t>
+  </si>
+  <si>
+    <t>Ausy</t>
+  </si>
+  <si>
+    <t>Stage pour ETIX</t>
+  </si>
+  <si>
+    <t>jai jamais répondu</t>
+  </si>
+  <si>
+    <t>Conception d'une veste informatisée modulaire (h/f)</t>
+  </si>
+  <si>
+    <t>Atos</t>
+  </si>
+  <si>
+    <t>Ingénieur électrotechnique</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>Conception Banc Electro Hydro</t>
+  </si>
+  <si>
+    <t>Etude de système électronique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,27 +511,63 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -470,30 +575,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="60 % - Accent4" xfId="5" builtinId="44"/>
+    <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutre" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -518,6 +674,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -529,6 +696,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I54" totalsRowShown="0">
+  <autoFilter ref="A1:I54">
+    <filterColumn colId="8"/>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Entreprise" dataDxfId="5" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="2" name="offre"/>
+    <tableColumn id="3" name="date" dataDxfId="4"/>
+    <tableColumn id="4" name="relance"/>
+    <tableColumn id="5" name="reponse"/>
+    <tableColumn id="6" name="Entretien"/>
+    <tableColumn id="7" name="remarque "/>
+    <tableColumn id="8" name="contact" dataDxfId="3" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="9" name="Avis"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -996,21 +1183,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G1" t="s">
         <v>23</v>
@@ -1035,134 +1225,155 @@
       <c r="H1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="I1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="13">
+        <v>42379</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="1">
         <v>42373</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C5" s="9">
         <v>42374</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
+    <row r="6" spans="1:9">
+      <c r="A6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C6" s="13">
         <v>42375</v>
       </c>
-      <c r="E4" s="1">
+      <c r="D6" s="12"/>
+      <c r="E6" s="13">
         <v>42375</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1">
-        <v>42375</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1">
-        <v>42375</v>
+      <c r="F6" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="H6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="I6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9">
         <v>42375</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
       </c>
       <c r="H7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1">
         <v>42375</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>42375</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
@@ -1171,83 +1382,83 @@
         <v>42375</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1">
-        <v>42376</v>
+        <v>42375</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1">
-        <v>42376</v>
+        <v>42375</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1">
         <v>42376</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1">
         <v>42376</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -1255,213 +1466,229 @@
       <c r="C15" s="1">
         <v>42376</v>
       </c>
-      <c r="E15" s="1">
-        <v>42377</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="G15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42376</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="11">
+        <v>42376</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="I17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="C18" s="11">
         <v>42379</v>
       </c>
-      <c r="E16" s="1">
-        <v>42380</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="1">
-        <v>42379</v>
-      </c>
-      <c r="E17" s="1">
-        <v>42385</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="1">
-        <v>42379</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="I18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="13">
         <v>42379</v>
       </c>
-      <c r="E19" s="1">
-        <v>42382</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>116</v>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13">
+        <v>42385</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1">
         <v>42379</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
       <c r="H20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="1">
+    <row r="21" spans="1:9">
+      <c r="A21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="9">
         <v>42379</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9">
+        <v>42382</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="1">
+    <row r="22" spans="1:9">
+      <c r="A22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="9">
         <v>42379</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="1"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1">
-        <v>42380</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>42379</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="1">
-        <v>42380</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="13">
+        <v>42379</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42380</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="1">
-        <v>42381</v>
-      </c>
-      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1">
         <v>42380</v>
@@ -1469,61 +1696,67 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1">
-        <v>42380</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>42381</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42381</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="5" t="s">
-        <v>78</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="21">
+        <v>42380</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
-        <v>42381</v>
+        <v>42380</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
@@ -1531,86 +1764,98 @@
       <c r="C30" s="1">
         <v>42381</v>
       </c>
-      <c r="E30" s="1">
-        <v>42387</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>96</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1">
         <v>42381</v>
       </c>
-      <c r="E31" s="1">
-        <v>42389</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B32" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="H31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="13">
         <v>42381</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="1"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13">
+        <v>42387</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="1">
-        <v>42382</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="11">
+        <v>42381</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="1">
-        <v>42382</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="9">
+        <v>42381</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
@@ -1618,202 +1863,386 @@
       <c r="C35" s="1">
         <v>42382</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
         <v>42382</v>
       </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="A37" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="9">
         <v>42382</v>
       </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C38" s="1">
-        <v>42383</v>
+        <v>42382</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" t="s">
-        <v>110</v>
-      </c>
-      <c r="C39" s="1">
-        <v>42383</v>
-      </c>
-      <c r="E39" s="1">
-        <v>42387</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="A39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="9">
+        <v>42382</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="2" t="s">
-        <v>111</v>
+      <c r="A40" t="s">
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1">
         <v>42383</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" s="1">
+      <c r="A41" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="13">
+        <v>42383</v>
+      </c>
+      <c r="D41" s="12"/>
+      <c r="E41" s="13">
         <v>42387</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="F41" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1">
-        <v>42387</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>42383</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1">
+        <v>42387</v>
+      </c>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="9">
+        <v>42387</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="1">
+        <v>42395</v>
+      </c>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" t="s">
         <v>125</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C46" s="1">
+        <v>42388</v>
+      </c>
+      <c r="E46" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="13">
+        <v>42388</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13">
+        <v>42388</v>
+      </c>
+      <c r="F48" t="s">
+        <v>114</v>
+      </c>
+      <c r="H48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="7">
+        <v>42025</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="19">
+        <v>42390</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="5"/>
+      <c r="I50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="7">
+        <v>42394</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" s="7">
+        <v>42395</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="7">
+        <v>42395</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="7">
+        <v>42395</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="1">
-        <v>42388</v>
-      </c>
-      <c r="E43" t="s">
-        <v>130</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" t="s">
-        <v>127</v>
-      </c>
-      <c r="C45" s="1">
-        <v>42388</v>
-      </c>
-      <c r="E45" s="1">
-        <v>42388</v>
-      </c>
-      <c r="F45" t="s">
-        <v>131</v>
-      </c>
-      <c r="H45" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>79</v>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F47:F1048576 F1:F45">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"POTENTIEL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"OUI"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$F$5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G11" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="H14" r:id="rId3" tooltip="Postulez en ligne !" display="mailto:recrutement@basystemes.fr"/>
-    <hyperlink ref="G14" r:id="rId4"/>
-    <hyperlink ref="H3" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G9" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8" display="rh.faverges@staubli.com"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
-    <hyperlink ref="G15" r:id="rId11"/>
-    <hyperlink ref="A29" r:id="rId12" display="mailto:jobs@sen.se"/>
-    <hyperlink ref="H28" r:id="rId13"/>
-    <hyperlink ref="H29" r:id="rId14"/>
-    <hyperlink ref="H27" r:id="rId15"/>
-    <hyperlink ref="H30" r:id="rId16"/>
-    <hyperlink ref="H25" r:id="rId17"/>
-    <hyperlink ref="H40" r:id="rId18"/>
-    <hyperlink ref="H44" r:id="rId19" display="javascript: WebMail('vreynes@oet.fr','')"/>
-    <hyperlink ref="H43" r:id="rId20"/>
+    <hyperlink ref="G13" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="H16" r:id="rId3" tooltip="Postulez en ligne !" display="mailto:recrutement@basystemes.fr"/>
+    <hyperlink ref="G16" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="G10" r:id="rId6"/>
+    <hyperlink ref="G11" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8" display="rh.faverges@staubli.com"/>
+    <hyperlink ref="G14" r:id="rId9"/>
+    <hyperlink ref="G15" r:id="rId10"/>
+    <hyperlink ref="G17" r:id="rId11"/>
+    <hyperlink ref="A31" r:id="rId12" display="mailto:jobs@sen.se"/>
+    <hyperlink ref="H30" r:id="rId13"/>
+    <hyperlink ref="H31" r:id="rId14"/>
+    <hyperlink ref="H29" r:id="rId15"/>
+    <hyperlink ref="H32" r:id="rId16"/>
+    <hyperlink ref="H27" r:id="rId17"/>
+    <hyperlink ref="H42" r:id="rId18"/>
+    <hyperlink ref="H47" r:id="rId19" display="javascript: WebMail('vreynes@oet.fr','')"/>
+    <hyperlink ref="H46" r:id="rId20"/>
+    <hyperlink ref="H49" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
+  <tableParts count="1">
+    <tablePart r:id="rId23"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>